<commit_message>
Hybrid framework Vrsion 1.2
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestData.xlsx
+++ b/src/main/java/testData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -84,9 +84,6 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>iMacs</t>
   </si>
   <si>
@@ -99,64 +96,55 @@
     <t>22, LimeSquare, City Road</t>
   </si>
   <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Wasey</t>
+  </si>
+  <si>
+    <t>Wazed</t>
+  </si>
+  <si>
+    <t>waseyrabby@btinternet.com</t>
+  </si>
+  <si>
+    <t>waseyraby@gmail.com</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>hot</t>
+  </si>
+  <si>
+    <t>akm</t>
+  </si>
+  <si>
+    <t>wazed</t>
+  </si>
+  <si>
+    <t>3306 35th ave</t>
+  </si>
+  <si>
+    <t>astoria</t>
+  </si>
+  <si>
+    <t>HomeTest</t>
+  </si>
+  <si>
+    <t>SmokeTest</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>RegistrationTest</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Wasey</t>
-  </si>
-  <si>
-    <t>Wazed</t>
-  </si>
-  <si>
-    <t>waseyrabby</t>
-  </si>
-  <si>
-    <t>718756home</t>
-  </si>
-  <si>
-    <t>waseyrabby@btinternet.com</t>
-  </si>
-  <si>
-    <t>waseyraby@gmail.com</t>
-  </si>
-  <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
-    <t>wasey</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>hot</t>
-  </si>
-  <si>
-    <t>akm</t>
-  </si>
-  <si>
-    <t>wazed</t>
-  </si>
-  <si>
-    <t>3306 35th ave</t>
-  </si>
-  <si>
-    <t>astoria</t>
-  </si>
-  <si>
-    <t>CheckoutTest</t>
-  </si>
-  <si>
-    <t>HomeTest</t>
-  </si>
-  <si>
-    <t>SmokeTest</t>
-  </si>
-  <si>
-    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -164,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,6 +176,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,15 +313,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -363,13 +363,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
@@ -1033,24 +1040,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.6640625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="19.5" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="17.5" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="14.5" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="12.6640625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="36.6640625" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="29.1640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20" customHeight="1">
@@ -1099,16 +1108,16 @@
     </row>
     <row r="2" spans="1:14" ht="20" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="11">
+        <v>718756</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>15</v>
@@ -1120,7 +1129,7 @@
         <v>17</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>18</v>
@@ -1129,45 +1138,45 @@
         <v>19</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="11">
         <v>7777777777</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="20" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11">
+        <v>718756</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>19</v>
@@ -1179,60 +1188,58 @@
         <v>7777777777</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:14" ht="20" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="11">
         <v>718756</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="K4" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L4" s="11">
         <v>9083277874</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" ht="20" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="11">
         <v>718756</v>
@@ -1241,37 +1248,39 @@
         <v>14</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L5" s="11">
         <v>9083277874</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1">
       <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
+      <c r="B6" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -1864,15 +1873,23 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Test@123"/>
-    <hyperlink ref="C3" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="M3" r:id="rId3"/>
-    <hyperlink ref="M2" r:id="rId4"/>
-    <hyperlink ref="M5" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6"/>
+    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink ref="M2" r:id="rId3"/>
+    <hyperlink ref="M5" r:id="rId4"/>
+    <hyperlink ref="M4" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6" display="Test@123"/>
+    <hyperlink ref="C4" r:id="rId7" display="Test@123"/>
+    <hyperlink ref="C5" r:id="rId8" display="Test@123"/>
+    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId10"/>
+    <hyperlink ref="B3" r:id="rId11"/>
+    <hyperlink ref="B4" r:id="rId12"/>
+    <hyperlink ref="B5" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>